<commit_message>
Aula 24-11 pos aula
</commit_message>
<xml_diff>
--- a/Professor/Plano de Aulas.xlsx
+++ b/Professor/Plano de Aulas.xlsx
@@ -15,7 +15,6 @@
     <sheet name="plano de aula" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -765,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +837,7 @@
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I4" t="s">
@@ -873,7 +872,7 @@
       <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M5" t="s">
@@ -896,7 +895,7 @@
       <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I6" t="s">
@@ -925,13 +924,13 @@
       <c r="E7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I7" t="s">
         <v>42</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="3" t="s">
         <v>43</v>
       </c>
       <c r="M7" t="s">
@@ -957,7 +956,7 @@
       <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>51</v>
       </c>
       <c r="K8" t="s">
@@ -1127,7 +1126,7 @@
       <c r="C15" t="s">
         <v>102</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="3" t="s">
         <v>103</v>
       </c>
       <c r="K15" t="s">
@@ -1161,7 +1160,7 @@
       <c r="A17" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>113</v>
       </c>
       <c r="I17" t="s">

</xml_diff>